<commit_message>
cleaned up redundant files
</commit_message>
<xml_diff>
--- a/some_test_results.xlsx
+++ b/some_test_results.xlsx
@@ -116,10 +116,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -149,7 +149,136 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,135 +287,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,67 +324,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,114 +505,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,25 +519,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,17 +548,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -587,11 +572,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -615,20 +606,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -638,134 +638,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -781,18 +781,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -812,9 +806,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1144,7 +1135,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1237,10 +1228,10 @@
       <c r="G3" s="4">
         <v>0.0746</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>0.1116</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <v>0.117</v>
       </c>
       <c r="J3" s="4">
@@ -1252,22 +1243,22 @@
       <c r="L3" s="4">
         <v>0.1171</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <v>0.1183</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="5">
         <f t="shared" ref="N3:N14" si="0">AVERAGE(H3:M3)</f>
         <v>0.1164</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="12">
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="10">
         <v>0.12255</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="10">
         <v>0.11987</v>
       </c>
-      <c r="S3" s="13"/>
+      <c r="S3" s="11"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
@@ -1283,43 +1274,43 @@
         <v>53</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>0.1112</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>0.0781</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0.1132</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>0.1171</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>0.1176</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>0.1169</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>0.1174</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>0.1183</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <f t="shared" si="0"/>
         <v>0.11675</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="6">
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="5">
         <v>0.12272</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="5">
         <v>0.12084</v>
       </c>
-      <c r="S4" s="13"/>
+      <c r="S4" s="11"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
@@ -1335,43 +1326,43 @@
         <v>53</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>0.1136</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>0.0752</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>0.1152</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>0.1186</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>0.1176</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>0.1173</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>0.1186</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>0.1194</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <f t="shared" si="0"/>
         <v>0.117783333333333</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6">
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="5">
         <v>0.12094</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="5">
         <v>0.11986</v>
       </c>
-      <c r="S5" s="13"/>
+      <c r="S5" s="11"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="3" t="s">
@@ -1411,17 +1402,17 @@
       <c r="M6" s="4">
         <v>0.118</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="5">
         <f t="shared" si="0"/>
         <v>0.11545</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="12">
+      <c r="R6" s="10">
         <v>0.11787</v>
       </c>
-      <c r="S6" s="13"/>
+      <c r="S6" s="11"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
@@ -1437,41 +1428,41 @@
         <v>100</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>0.1104</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>0.0666</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>0.1129</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>0.1159</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>0.1162</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>0.1153</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>0.116</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <v>0.1184</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="5">
         <f t="shared" si="0"/>
         <v>0.115783333333333</v>
       </c>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6">
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5">
         <v>0.11737</v>
       </c>
-      <c r="S7" s="13"/>
+      <c r="S7" s="11"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
@@ -1511,17 +1502,17 @@
       <c r="M8" s="4">
         <v>0.118</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="5">
         <f t="shared" si="0"/>
         <v>0.115416666666667</v>
       </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="12">
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="10">
         <v>0.11792</v>
       </c>
-      <c r="S8" s="13"/>
+      <c r="S8" s="11"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
@@ -1561,125 +1552,125 @@
       <c r="M9" s="4">
         <v>0.1177</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <f t="shared" si="0"/>
         <v>0.115833333333333</v>
       </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="12">
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="10">
         <v>0.11827</v>
       </c>
-      <c r="S9" s="13"/>
+      <c r="S9" s="11"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>41</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>600</v>
       </c>
       <c r="D10" s="3">
         <v>100</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>0.1103</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>0.0708</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>0.1133</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>0.1159</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>0.1162</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>0.1153</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <v>0.116</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="5">
         <v>0.1184</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="5">
         <f t="shared" si="0"/>
         <v>0.11585</v>
       </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6">
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5">
         <v>0.11749</v>
       </c>
-      <c r="S10" s="13"/>
+      <c r="S10" s="11"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>41</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>60</v>
       </c>
       <c r="D11" s="3">
         <v>100</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>0.1119</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>0.0701</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>0.1166</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>0.1165</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>0.1162</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>0.1153</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <v>0.116</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="5">
         <v>0.1199</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="5">
         <f t="shared" si="0"/>
         <v>0.11675</v>
       </c>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5">
         <v>0.1184</v>
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>41</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>3600</v>
       </c>
       <c r="D12" s="3">
@@ -1710,25 +1701,25 @@
       <c r="M12" s="4">
         <v>0.1187</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="5">
         <f t="shared" si="0"/>
         <v>0.115966666666667</v>
       </c>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="14">
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="12">
         <v>0.11835</v>
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>16</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>1800</v>
       </c>
       <c r="D13" s="4">
@@ -1759,25 +1750,25 @@
       <c r="M13" s="4">
         <v>0.1213</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="5">
         <f t="shared" si="0"/>
         <v>0.117966666666667</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="15">
+      <c r="R13" s="13">
         <v>0.11711</v>
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>0</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>1800</v>
       </c>
       <c r="D14" s="3">
@@ -1808,14 +1799,14 @@
       <c r="M14" s="4">
         <v>0.1202</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="5">
         <f t="shared" si="0"/>
         <v>0.118066666666667</v>
       </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="14">
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="12">
         <v>0.11803</v>
       </c>
     </row>
@@ -1832,39 +1823,39 @@
       <c r="D15" s="3">
         <v>100</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10">
+      <c r="E15" s="7"/>
+      <c r="F15" s="8">
         <v>0.1249</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="9">
         <v>0.073</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="9">
         <v>0.113</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="9">
         <v>0.1149</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="9">
         <v>0.1162</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="9">
         <v>0.115</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="9">
         <v>0.1162</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="9">
         <v>0.1181</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="7">
         <f>MIN(N7:N9)</f>
         <v>0.115416666666667</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="16">
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="12">
         <v>0.11833</v>
       </c>
     </row>
@@ -1874,19 +1865,19 @@
       </c>
     </row>
     <row r="21" spans="18:18">
-      <c r="R21" s="12"/>
+      <c r="R21" s="10"/>
     </row>
     <row r="22" spans="18:18">
-      <c r="R22" s="6"/>
+      <c r="R22" s="5"/>
     </row>
     <row r="23" spans="18:18">
-      <c r="R23" s="12"/>
+      <c r="R23" s="10"/>
     </row>
     <row r="24" spans="18:18">
-      <c r="R24" s="12"/>
+      <c r="R24" s="10"/>
     </row>
     <row r="25" spans="18:18">
-      <c r="R25" s="16"/>
+      <c r="R25" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:R15">

</xml_diff>